<commit_message>
Using appsettings.json and update unit test
</commit_message>
<xml_diff>
--- a/TonicCertificateGenerator/contact.xlsx
+++ b/TonicCertificateGenerator/contact.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\pierr\Projet\TONIC-certificate-generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\pierr\Projet\TONIC-certificate-generator\TonicCertificateGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50C8F90-6251-4363-BA01-3F7DD67C0B90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EFC35E-0BC9-45D7-9866-596BC3FC3B81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="345" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,22 +36,22 @@
     <t>email</t>
   </si>
   <si>
-    <t>pierre</t>
-  </si>
-  <si>
-    <t>vanobbergen</t>
-  </si>
-  <si>
     <t>pierrevob@hotmail.com</t>
   </si>
   <si>
-    <t>melvin</t>
-  </si>
-  <si>
     <t>melvin.leble@supinfo.com</t>
   </si>
   <si>
-    <t>leble</t>
+    <t>Pierre</t>
+  </si>
+  <si>
+    <t>Vanobbergen</t>
+  </si>
+  <si>
+    <t>Melvin</t>
+  </si>
+  <si>
+    <t>Leble</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,24 +404,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Inventory Manager for serialnumber
</commit_message>
<xml_diff>
--- a/TonicCertificateGenerator/contact.xlsx
+++ b/TonicCertificateGenerator/contact.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\pierr\Projet\TONIC-certificate-generator\TonicCertificateGenerator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUPINFO\STAGE\TonicTeaching\TONIC-certificate-generator\TonicCertificateGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EFC35E-0BC9-45D7-9866-596BC3FC3B81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9B0A10-F295-4BFC-8E9B-E0D8A0799D0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="345" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>firstname</t>
   </si>
@@ -36,22 +36,19 @@
     <t>email</t>
   </si>
   <si>
-    <t>pierrevob@hotmail.com</t>
-  </si>
-  <si>
     <t>melvin.leble@supinfo.com</t>
   </si>
   <si>
-    <t>Pierre</t>
-  </si>
-  <si>
-    <t>Vanobbergen</t>
-  </si>
-  <si>
     <t>Melvin</t>
   </si>
   <si>
     <t>Leble</t>
+  </si>
+  <si>
+    <t>LEBLE</t>
+  </si>
+  <si>
+    <t>leble17@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -101,7 +98,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,15 +380,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,26 +399,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The application supports excel with 2 columns. Add unit tests for excel with 2 columns, 3 columns and excel with one contact. Conference date is generated from app.json and appear in output pdf
</commit_message>
<xml_diff>
--- a/TonicCertificateGenerator/contact.xlsx
+++ b/TonicCertificateGenerator/contact.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUPINFO\STAGE\TonicTeaching\TONIC-certificate-generator\TonicCertificateGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9B0A10-F295-4BFC-8E9B-E0D8A0799D0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EBF18D-3E33-48CC-843B-90C4A537A84D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2616" yWindow="2640" windowWidth="17112" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,30 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>melvin.leble@supinfo.com</t>
+    <t>sebastien.debeauffort@outlook.com</t>
   </si>
   <si>
-    <t>Melvin</t>
+    <t>names</t>
   </si>
   <si>
-    <t>Leble</t>
-  </si>
-  <si>
-    <t>LEBLE</t>
-  </si>
-  <si>
-    <t>leble17@gmail.com</t>
+    <t>Jean exemple</t>
   </si>
 </sst>
 </file>
@@ -377,55 +365,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{82FC22B9-F20E-48D7-AC72-6BF54D0E3313}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{32E4B448-C007-4B00-B411-A33F2B5FDFAF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add readme, email error filter, exception handler. Add a Serilog config in appsettings.json. Reorganize code in units tests.
</commit_message>
<xml_diff>
--- a/TonicCertificateGenerator/contact.xlsx
+++ b/TonicCertificateGenerator/contact.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUPINFO\STAGE\TonicTeaching\TONIC-certificate-generator\TonicCertificateGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EBF18D-3E33-48CC-843B-90C4A537A84D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F029E414-BB94-4F0B-8D87-FFBD3EC44454}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2616" yWindow="2640" windowWidth="17112" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>sebastien.debeauffort@outlook.com</t>
-  </si>
-  <si>
     <t>names</t>
   </si>
   <si>
     <t>Jean exemple</t>
+  </si>
+  <si>
+    <t>jeanexemple@outlook.com</t>
+  </si>
+  <si>
+    <t>Jean exemple2</t>
+  </si>
+  <si>
+    <t>jeanexemple2@outlook.com</t>
+  </si>
+  <si>
+    <t>Jean exemple3</t>
+  </si>
+  <si>
+    <t>jeanéxemple3@outlook.com</t>
+  </si>
+  <si>
+    <t>Jean exemple4</t>
+  </si>
+  <si>
+    <t>jeanexemple 4@outlook.com</t>
+  </si>
+  <si>
+    <t>Jeanexemple5</t>
+  </si>
+  <si>
+    <t>jeanexemple5outlook.com</t>
+  </si>
+  <si>
+    <t>Jeanexemple6</t>
+  </si>
+  <si>
+    <t>jeanexemple6@outlookcom</t>
   </si>
 </sst>
 </file>
@@ -365,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,7 +409,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -387,13 +417,61 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{8C5F340E-38FF-4FE3-9C32-58AE8B68E1EE}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{32BBF278-2DFC-4D33-A7FE-574108EEAFE7}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{15DA699D-723D-4710-B5DF-95CBF7E2972C}"/>
+    <hyperlink ref="B5" r:id="rId4" display="jeanexemple2@outlook.com" xr:uid="{F2D999C4-859F-4933-A29B-2B3010A61F58}"/>
+    <hyperlink ref="B6" r:id="rId5" display="jeanexemple5@outlook.com" xr:uid="{F749E320-7BA1-434E-8B28-2590BF0BF062}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{629DD1CC-E466-4911-8F5E-A048BEC46AE1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>